<commit_message>
Adding the specifications and write-up
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr date1904="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="36" windowWidth="15960" windowHeight="13176"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1 - Crossover (Strassen)" sheetId="1" r:id="rId4"/>
-    <sheet name="Sheet 1-1 - Crossover (Regular)" sheetId="2" r:id="rId5"/>
-    <sheet name="Sheet 2" sheetId="3" r:id="rId6"/>
+    <sheet name="Sheet 1 - Crossover (Strassen)" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet 1-1 - Crossover (Regular)" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet 2" sheetId="3" r:id="rId3"/>
   </sheets>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>Crossover (Strassen)</t>
   </si>
@@ -24,7 +26,6 @@
   <si>
     <t>Crossover (Regular)</t>
   </si>
-  <si/>
   <si>
     <t>Strassen</t>
   </si>
@@ -41,12 +42,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="0" formatCode="General"/>
-    <numFmt numFmtId="59" formatCode="0.00000"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -58,7 +58,7 @@
       <name val="Helvetica"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica"/>
@@ -204,55 +204,55 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="15">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="59" fontId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="59" fontId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="59" fontId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="59" fontId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -262,32 +262,86 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="ff3f3f3f"/>
-      <rgbColor rgb="ffdbdbdb"/>
-      <rgbColor rgb="ffb8b8b8"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ff557690"/>
-      <rgbColor rgb="ff5a704d"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFBDC0BF"/>
+      <rgbColor rgb="FFA5A5A5"/>
+      <rgbColor rgb="FF3F3F3F"/>
+      <rgbColor rgb="FFDBDBDB"/>
+      <rgbColor rgb="FFB8B8B8"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FF557690"/>
+      <rgbColor rgb="FF5A704D"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
+  <c:style val="2"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -296,7 +350,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" i="0" strike="noStrike" sz="1200" u="none">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -304,7 +358,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="0" i="0" strike="noStrike" sz="1200" u="none">
+              <a:rPr sz="1200" b="0" i="0" u="none" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -319,10 +373,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.140228"/>
+          <c:x val="0.14022799999999999"/>
           <c:y val="0"/>
-          <c:w val="0.719543"/>
-          <c:h val="0.0846906"/>
+          <c:w val="0.71954300000000004"/>
+          <c:h val="8.4690600000000005E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -331,17 +385,17 @@
         <a:effectLst/>
       </c:spPr>
     </c:title>
-    <c:autoTitleDeleted val="1"/>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.153787"/>
-          <c:y val="0.0846906"/>
-          <c:w val="0.825288"/>
-          <c:h val="0.790432"/>
+          <c:x val="0.15378700000000001"/>
+          <c:y val="8.4690600000000005E-2"/>
+          <c:w val="0.82528800000000002"/>
+          <c:h val="0.79043200000000002"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -362,9 +416,6 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF"/>
-            </a:solidFill>
             <a:ln w="50800" cap="flat">
               <a:solidFill>
                 <a:srgbClr val="567691"/>
@@ -391,35 +442,11 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:dLbls>
-            <c:numFmt formatCode="#,##0" sourceLinked="1"/>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" i="0" strike="noStrike" sz="1200" u="none">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Helvetica"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="t"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>'Sheet 2'!$B$1:$I$1</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>60</c:v>
@@ -445,37 +472,38 @@
                 <c:pt idx="7">
                   <c:v>67</c:v>
                 </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'Sheet 2'!$B$4:$I$4</c:f>
               <c:numCache>
+                <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1.072855</c:v>
+                  <c:v>1.0728546239325933</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.061954</c:v>
+                  <c:v>1.0619539026088283</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.045770</c:v>
+                  <c:v>1.0457701202129144</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.058082</c:v>
+                  <c:v>1.0580822264987588</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.947813</c:v>
+                  <c:v>0.94781341416508169</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.947620</c:v>
+                  <c:v>0.94761998047054996</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.949816</c:v>
+                  <c:v>0.94981612930813297</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.950642</c:v>
+                  <c:v>0.95064175830148823</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -497,9 +525,6 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF"/>
-            </a:solidFill>
             <a:ln w="50800" cap="flat">
               <a:solidFill>
                 <a:srgbClr val="5B704E"/>
@@ -513,50 +538,12 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
-            <c:size val="4"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-              <a:ln w="50800" cap="flat">
-                <a:solidFill>
-                  <a:srgbClr val="5B704E"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-                <a:miter lim="400000"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
           </c:marker>
-          <c:dLbls>
-            <c:numFmt formatCode="#,##0" sourceLinked="1"/>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" i="0" strike="noStrike" sz="1200" u="none">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Helvetica"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="t"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>'Sheet 2'!$B$1:$I$1</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>60</c:v>
@@ -582,49 +569,59 @@
                 <c:pt idx="7">
                   <c:v>67</c:v>
                 </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'Sheet 2'!$B$5:$I$5</c:f>
               <c:numCache>
+                <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1.000000</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.000000</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.000000</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.000000</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.000000</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.000000</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.000000</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.000000</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="2094734552"/>
-        <c:axId val="2094734553"/>
+        <c:smooth val="0"/>
+        <c:axId val="48030464"/>
+        <c:axId val="48032384"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2094734552"/>
+        <c:axId val="48030464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -637,7 +634,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" i="0" strike="noStrike" sz="1100" u="none">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -645,7 +642,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0" i="0" strike="noStrike" sz="1100" u="none">
+                  <a:rPr sz="1100" b="0" i="0" u="none" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -656,7 +653,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="1"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -679,23 +675,25 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" i="0" strike="noStrike" sz="1000" u="none">
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
                 <a:latin typeface="Helvetica"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2094734553"/>
+        <c:crossAx val="48032384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2094734553"/>
+        <c:axId val="48032384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -719,7 +717,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" i="0" strike="noStrike" sz="1100" u="none">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -727,7 +725,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0" i="0" strike="noStrike" sz="1100" u="none">
+                  <a:rPr sz="1100" b="0" i="0" u="none" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -738,10 +736,9 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="1"/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -759,20 +756,21 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" i="0" strike="noStrike" sz="1000" u="none">
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
                 <a:latin typeface="Helvetica"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2094734552"/>
+        <c:crossAx val="48030464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="0.075"/>
-        <c:minorUnit val="0.0375"/>
+        <c:majorUnit val="7.4999999999999997E-2"/>
+        <c:minorUnit val="3.7499999999999999E-2"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -785,6 +783,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
   <c:spPr>
     <a:noFill/>
@@ -793,11 +792,16 @@
     </a:ln>
     <a:effectLst/>
   </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
@@ -811,18 +815,18 @@
       <xdr:row>25</xdr:row>
       <xdr:rowOff>82474</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="3592537" y="2426258"/>
-        <a:ext cx="5462564" cy="3898901"/>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
       </xdr:xfrm>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -832,7 +836,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Blank">
   <a:themeElements>
     <a:clrScheme name="Blank">
       <a:dk1>
@@ -958,7 +962,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -967,7 +971,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -976,7 +980,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -1040,8 +1044,8 @@
     <a:spDef>
       <a:spPr>
         <a:blipFill rotWithShape="1">
-          <a:blip r:embed="rId1"/>
-          <a:srcRect l="0" t="0" r="0" b="0"/>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+          <a:srcRect/>
           <a:tile tx="0" ty="0" sx="100000" sy="100000" flip="none" algn="tl"/>
         </a:blipFill>
         <a:ln w="12700" cap="flat">
@@ -1049,7 +1053,7 @@
           <a:miter lim="400000"/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+          <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
             <a:srgbClr val="000000">
               <a:alpha val="50000"/>
             </a:srgbClr>
@@ -1057,7 +1061,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1076,7 +1080,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1200" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1084,7 +1088,7 @@
               <a:srgbClr val="FFFFFF"/>
             </a:solidFill>
             <a:effectLst>
-              <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="25400" dist="23998" dir="2700000">
+              <a:outerShdw blurRad="25400" dist="23998" dir="2700000" rotWithShape="0">
                 <a:srgbClr val="000000">
                   <a:alpha val="31034"/>
                 </a:srgbClr>
@@ -1112,7 +1116,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1138,7 +1142,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1164,7 +1168,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1190,7 +1194,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1216,7 +1220,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1242,7 +1246,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1268,7 +1272,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1294,7 +1298,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1320,7 +1324,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1333,9 +1337,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -1352,7 +1362,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1371,7 +1381,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1397,7 +1407,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1423,7 +1433,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1449,7 +1459,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1475,7 +1485,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1501,7 +1511,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1527,7 +1537,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1553,7 +1563,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1579,7 +1589,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1605,7 +1615,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1618,9 +1628,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1634,7 +1650,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1653,7 +1669,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1683,7 +1699,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1709,7 +1725,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1735,7 +1751,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1761,7 +1777,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1787,7 +1803,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1813,7 +1829,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1839,7 +1855,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1865,7 +1881,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1891,7 +1907,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1904,283 +1920,284 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:I9"/>
+  <dimension ref="A1:IV9"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.3516" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.3516" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.3516" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.3516" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.3516" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.3516" style="1" customWidth="1"/>
-    <col min="7" max="7" width="16.3516" style="1" customWidth="1"/>
-    <col min="8" max="8" width="16.3516" style="1" customWidth="1"/>
-    <col min="9" max="9" width="16.3516" style="1" customWidth="1"/>
-    <col min="10" max="256" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="256" width="16.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="28" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:9" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
     </row>
-    <row r="2" ht="20.55" customHeight="1">
-      <c r="A2" t="s" s="3">
+    <row r="2" spans="1:9" ht="20.55" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="3">
         <v>60</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>61</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="3">
         <v>62</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="3">
         <v>63</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="3">
         <v>64</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="3">
         <v>65</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="3">
         <v>66</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2" s="3">
         <v>67</v>
       </c>
     </row>
-    <row r="3" ht="21.55" customHeight="1">
-      <c r="A3" s="5">
+    <row r="3" spans="1:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
         <v>16</v>
       </c>
-      <c r="B3" s="6">
-        <v>0.0006980000000000007</v>
-      </c>
-      <c r="C3" s="7">
-        <v>0.0006940000000000002</v>
-      </c>
-      <c r="D3" s="7">
-        <v>0.0006949999999999977</v>
-      </c>
-      <c r="E3" s="7">
-        <v>0.0007049999999999973</v>
-      </c>
-      <c r="F3" s="7">
-        <v>0.000671999999999999</v>
-      </c>
-      <c r="G3" s="7">
-        <v>0.000674000000000001</v>
-      </c>
-      <c r="H3" s="7">
-        <v>0.000673</v>
-      </c>
-      <c r="I3" s="7">
-        <v>0.0006919999999999982</v>
+      <c r="B3" s="5">
+        <v>6.980000000000007E-4</v>
+      </c>
+      <c r="C3" s="6">
+        <v>6.9400000000000017E-4</v>
+      </c>
+      <c r="D3" s="6">
+        <v>6.949999999999977E-4</v>
+      </c>
+      <c r="E3" s="6">
+        <v>7.049999999999973E-4</v>
+      </c>
+      <c r="F3" s="6">
+        <v>6.7199999999999899E-4</v>
+      </c>
+      <c r="G3" s="6">
+        <v>6.7400000000000099E-4</v>
+      </c>
+      <c r="H3" s="6">
+        <v>6.7299999999999999E-4</v>
+      </c>
+      <c r="I3" s="6">
+        <v>6.9199999999999817E-4</v>
       </c>
     </row>
-    <row r="4" ht="21.35" customHeight="1">
-      <c r="A4" s="8">
+    <row r="4" spans="1:9" ht="21.3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
         <v>32</v>
       </c>
-      <c r="B4" s="9">
-        <v>0.004628</v>
-      </c>
-      <c r="C4" s="10">
-        <v>0.004615000000000001</v>
-      </c>
-      <c r="D4" s="10">
-        <v>0.004598000000000001</v>
-      </c>
-      <c r="E4" s="10">
-        <v>0.004768000000000001</v>
-      </c>
-      <c r="F4" s="10">
-        <v>0.004617</v>
-      </c>
-      <c r="G4" s="10">
-        <v>0.004660000000000001</v>
-      </c>
-      <c r="H4" s="10">
-        <v>0.004803000000000002</v>
-      </c>
-      <c r="I4" s="10">
-        <v>0.004872000000000001</v>
+      <c r="B4" s="8">
+        <v>4.6280000000000002E-3</v>
+      </c>
+      <c r="C4" s="9">
+        <v>4.615000000000001E-3</v>
+      </c>
+      <c r="D4" s="9">
+        <v>4.5980000000000014E-3</v>
+      </c>
+      <c r="E4" s="9">
+        <v>4.7680000000000014E-3</v>
+      </c>
+      <c r="F4" s="9">
+        <v>4.6169999999999996E-3</v>
+      </c>
+      <c r="G4" s="9">
+        <v>4.6600000000000009E-3</v>
+      </c>
+      <c r="H4" s="9">
+        <v>4.8030000000000017E-3</v>
+      </c>
+      <c r="I4" s="9">
+        <v>4.8720000000000013E-3</v>
       </c>
     </row>
-    <row r="5" ht="21.35" customHeight="1">
-      <c r="A5" s="8">
+    <row r="5" spans="1:9" ht="21.3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
         <v>64</v>
       </c>
-      <c r="B5" s="9">
-        <v>0.038587</v>
-      </c>
-      <c r="C5" s="10">
-        <v>0.038462</v>
-      </c>
-      <c r="D5" s="10">
-        <v>0.038509</v>
-      </c>
-      <c r="E5" s="10">
-        <v>0.03859199999999999</v>
-      </c>
-      <c r="F5" s="10">
-        <v>0.034324</v>
-      </c>
-      <c r="G5" s="10">
-        <v>0.035438</v>
-      </c>
-      <c r="H5" s="10">
-        <v>0.0339</v>
-      </c>
-      <c r="I5" s="10">
-        <v>0.033938</v>
+      <c r="B5" s="8">
+        <v>3.8587000000000003E-2</v>
+      </c>
+      <c r="C5" s="9">
+        <v>3.8462000000000003E-2</v>
+      </c>
+      <c r="D5" s="9">
+        <v>3.8509000000000002E-2</v>
+      </c>
+      <c r="E5" s="9">
+        <v>3.8591999999999987E-2</v>
+      </c>
+      <c r="F5" s="9">
+        <v>3.4324E-2</v>
+      </c>
+      <c r="G5" s="9">
+        <v>3.5437999999999997E-2</v>
+      </c>
+      <c r="H5" s="9">
+        <v>3.39E-2</v>
+      </c>
+      <c r="I5" s="9">
+        <v>3.3938000000000003E-2</v>
       </c>
     </row>
-    <row r="6" ht="21.35" customHeight="1">
-      <c r="A6" s="8">
+    <row r="6" spans="1:9" ht="21.3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
         <v>128</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="8">
         <v>0.288773</v>
       </c>
-      <c r="C6" s="10">
-        <v>0.286695</v>
-      </c>
-      <c r="D6" s="10">
-        <v>0.286646</v>
-      </c>
-      <c r="E6" s="10">
+      <c r="C6" s="9">
+        <v>0.28669499999999998</v>
+      </c>
+      <c r="D6" s="9">
+        <v>0.28664600000000001</v>
+      </c>
+      <c r="E6" s="9">
         <v>0.30179</v>
       </c>
-      <c r="F6" s="10">
-        <v>0.257307</v>
-      </c>
-      <c r="G6" s="10">
-        <v>0.255627</v>
-      </c>
-      <c r="H6" s="10">
-        <v>0.260514</v>
-      </c>
-      <c r="I6" s="10">
-        <v>0.258989</v>
+      <c r="F6" s="9">
+        <v>0.25730700000000001</v>
+      </c>
+      <c r="G6" s="9">
+        <v>0.25562699999999999</v>
+      </c>
+      <c r="H6" s="9">
+        <v>0.26051400000000002</v>
+      </c>
+      <c r="I6" s="9">
+        <v>0.25898900000000002</v>
       </c>
     </row>
-    <row r="7" ht="21.35" customHeight="1">
-      <c r="A7" s="8">
+    <row r="7" spans="1:9" ht="21.3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
         <v>256</v>
       </c>
-      <c r="B7" s="9">
-        <v>2.138107</v>
-      </c>
-      <c r="C7" s="10">
-        <v>2.117209</v>
-      </c>
-      <c r="D7" s="10">
-        <v>2.098275</v>
-      </c>
-      <c r="E7" s="10">
+      <c r="B7" s="8">
+        <v>2.1381070000000002</v>
+      </c>
+      <c r="C7" s="9">
+        <v>2.1172089999999999</v>
+      </c>
+      <c r="D7" s="9">
+        <v>2.0982750000000001</v>
+      </c>
+      <c r="E7" s="9">
         <v>2.104133</v>
       </c>
-      <c r="F7" s="10">
-        <v>1.880186</v>
-      </c>
-      <c r="G7" s="10">
+      <c r="F7" s="9">
+        <v>1.8801859999999999</v>
+      </c>
+      <c r="G7" s="9">
         <v>1.881707</v>
       </c>
-      <c r="H7" s="10">
-        <v>1.888054</v>
-      </c>
-      <c r="I7" s="10">
+      <c r="H7" s="9">
+        <v>1.8880539999999999</v>
+      </c>
+      <c r="I7" s="9">
         <v>1.88889</v>
       </c>
     </row>
-    <row r="8" ht="21.35" customHeight="1">
-      <c r="A8" s="8">
+    <row r="8" spans="1:9" ht="21.3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
         <v>512</v>
       </c>
-      <c r="B8" s="9">
-        <v>15.18387</v>
-      </c>
-      <c r="C8" s="10">
+      <c r="B8" s="8">
+        <v>15.183870000000001</v>
+      </c>
+      <c r="C8" s="9">
         <v>15.572607</v>
       </c>
-      <c r="D8" s="10">
-        <v>15.358704</v>
-      </c>
-      <c r="E8" s="10">
+      <c r="D8" s="9">
+        <v>15.358703999999999</v>
+      </c>
+      <c r="E8" s="9">
         <v>15.806412</v>
       </c>
-      <c r="F8" s="10">
-        <v>14.200722</v>
-      </c>
-      <c r="G8" s="10">
-        <v>13.79184</v>
-      </c>
-      <c r="H8" s="10">
-        <v>13.781123</v>
-      </c>
-      <c r="I8" s="10">
+      <c r="F8" s="9">
+        <v>14.200722000000001</v>
+      </c>
+      <c r="G8" s="9">
+        <v>13.791840000000001</v>
+      </c>
+      <c r="H8" s="9">
+        <v>13.781122999999999</v>
+      </c>
+      <c r="I8" s="9">
         <v>14.436073</v>
       </c>
     </row>
-    <row r="9" ht="21.35" customHeight="1">
-      <c r="A9" s="8">
+    <row r="9" spans="1:9" ht="21.3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
         <v>1024</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="8">
         <v>111.159296</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="9">
         <v>111.222448</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="9">
         <v>107.693055</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="9">
         <v>108.159448</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F9" s="9">
         <v>101.030027</v>
       </c>
-      <c r="G9" s="10">
+      <c r="G9" s="9">
         <v>100.579548</v>
       </c>
-      <c r="H9" s="10">
+      <c r="H9" s="9">
         <v>101.901027</v>
       </c>
-      <c r="I9" s="10">
+      <c r="I9" s="9">
         <v>103.202916</v>
       </c>
     </row>
@@ -2188,8 +2205,8 @@
   <mergeCells count="1">
     <mergeCell ref="A1:I1"/>
   </mergeCells>
-  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -2197,281 +2214,275 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:I9"/>
+  <dimension ref="A1:IV9"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.3516" style="11" customWidth="1"/>
-    <col min="2" max="2" width="16.3516" style="11" customWidth="1"/>
-    <col min="3" max="3" width="16.3516" style="11" customWidth="1"/>
-    <col min="4" max="4" width="16.3516" style="11" customWidth="1"/>
-    <col min="5" max="5" width="16.3516" style="11" customWidth="1"/>
-    <col min="6" max="6" width="16.3516" style="11" customWidth="1"/>
-    <col min="7" max="7" width="16.3516" style="11" customWidth="1"/>
-    <col min="8" max="8" width="16.3516" style="11" customWidth="1"/>
-    <col min="9" max="9" width="16.3516" style="11" customWidth="1"/>
-    <col min="10" max="256" width="16.3516" style="11" customWidth="1"/>
+    <col min="1" max="256" width="16.33203125" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="28" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:9" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
     </row>
-    <row r="2" ht="20.55" customHeight="1">
-      <c r="A2" t="s" s="3">
+    <row r="2" spans="1:9" ht="20.55" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="3">
         <v>60</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>61</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="3">
         <v>62</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="3">
         <v>63</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="3">
         <v>64</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="3">
         <v>65</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="3">
         <v>66</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2" s="3">
         <v>67</v>
       </c>
     </row>
-    <row r="3" ht="21.55" customHeight="1">
-      <c r="A3" s="5">
+    <row r="3" spans="1:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
         <v>16</v>
       </c>
-      <c r="B3" s="6">
-        <v>0.0006940000000000002</v>
-      </c>
-      <c r="C3" s="7">
-        <v>0.0006959999999999987</v>
-      </c>
-      <c r="D3" s="7">
-        <v>0.000674000000000001</v>
-      </c>
-      <c r="E3" s="7">
-        <v>0.0006910000000000006</v>
-      </c>
-      <c r="F3" s="7">
-        <v>0.0006940000000000002</v>
-      </c>
-      <c r="G3" s="7">
-        <v>0.0006899999999999996</v>
-      </c>
-      <c r="H3" s="7">
-        <v>0.0006940000000000002</v>
-      </c>
-      <c r="I3" s="7">
-        <v>0.0006689999999999995</v>
+      <c r="B3" s="5">
+        <v>6.9400000000000017E-4</v>
+      </c>
+      <c r="C3" s="6">
+        <v>6.959999999999987E-4</v>
+      </c>
+      <c r="D3" s="6">
+        <v>6.7400000000000099E-4</v>
+      </c>
+      <c r="E3" s="6">
+        <v>6.9100000000000064E-4</v>
+      </c>
+      <c r="F3" s="6">
+        <v>6.9400000000000017E-4</v>
+      </c>
+      <c r="G3" s="6">
+        <v>6.8999999999999964E-4</v>
+      </c>
+      <c r="H3" s="6">
+        <v>6.9400000000000017E-4</v>
+      </c>
+      <c r="I3" s="6">
+        <v>6.6899999999999946E-4</v>
       </c>
     </row>
-    <row r="4" ht="21.35" customHeight="1">
-      <c r="A4" s="8">
+    <row r="4" spans="1:9" ht="21.3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
         <v>32</v>
       </c>
-      <c r="B4" s="9">
-        <v>0.005649999999999999</v>
-      </c>
-      <c r="C4" s="10">
-        <v>0.005215000000000001</v>
-      </c>
-      <c r="D4" s="10">
-        <v>0.004664999999999999</v>
-      </c>
-      <c r="E4" s="10">
-        <v>0.004751999999999999</v>
-      </c>
-      <c r="F4" s="10">
-        <v>0.005489999999999998</v>
-      </c>
-      <c r="G4" s="10">
-        <v>0.005353999999999998</v>
-      </c>
-      <c r="H4" s="10">
-        <v>0.004623000000000002</v>
-      </c>
-      <c r="I4" s="10">
-        <v>0.004640999999999999</v>
+      <c r="B4" s="8">
+        <v>5.6499999999999988E-3</v>
+      </c>
+      <c r="C4" s="9">
+        <v>5.2150000000000009E-3</v>
+      </c>
+      <c r="D4" s="9">
+        <v>4.664999999999999E-3</v>
+      </c>
+      <c r="E4" s="9">
+        <v>4.7519999999999993E-3</v>
+      </c>
+      <c r="F4" s="9">
+        <v>5.4899999999999984E-3</v>
+      </c>
+      <c r="G4" s="9">
+        <v>5.3539999999999976E-3</v>
+      </c>
+      <c r="H4" s="9">
+        <v>4.6230000000000021E-3</v>
+      </c>
+      <c r="I4" s="9">
+        <v>4.6409999999999993E-3</v>
       </c>
     </row>
-    <row r="5" ht="21.35" customHeight="1">
-      <c r="A5" s="8">
+    <row r="5" spans="1:9" ht="21.3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
         <v>64</v>
       </c>
-      <c r="B5" s="9">
-        <v>0.033627</v>
-      </c>
-      <c r="C5" s="10">
-        <v>0.0336</v>
-      </c>
-      <c r="D5" s="10">
-        <v>0.033691</v>
-      </c>
-      <c r="E5" s="10">
-        <v>0.03351700000000001</v>
-      </c>
-      <c r="F5" s="10">
-        <v>0.033569</v>
-      </c>
-      <c r="G5" s="10">
-        <v>0.03401399999999999</v>
-      </c>
-      <c r="H5" s="10">
-        <v>0.033495</v>
-      </c>
-      <c r="I5" s="10">
-        <v>0.03385500000000001</v>
+      <c r="B5" s="8">
+        <v>3.3626999999999997E-2</v>
+      </c>
+      <c r="C5" s="9">
+        <v>3.3599999999999998E-2</v>
+      </c>
+      <c r="D5" s="9">
+        <v>3.3690999999999999E-2</v>
+      </c>
+      <c r="E5" s="9">
+        <v>3.3517000000000012E-2</v>
+      </c>
+      <c r="F5" s="9">
+        <v>3.3569000000000002E-2</v>
+      </c>
+      <c r="G5" s="9">
+        <v>3.4013999999999989E-2</v>
+      </c>
+      <c r="H5" s="9">
+        <v>3.3494999999999997E-2</v>
+      </c>
+      <c r="I5" s="9">
+        <v>3.385500000000001E-2</v>
       </c>
     </row>
-    <row r="6" ht="21.35" customHeight="1">
-      <c r="A6" s="8">
+    <row r="6" spans="1:9" ht="21.3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
         <v>128</v>
       </c>
-      <c r="B6" s="9">
-        <v>0.2536889999999999</v>
-      </c>
-      <c r="C6" s="10">
-        <v>0.253562</v>
-      </c>
-      <c r="D6" s="10">
+      <c r="B6" s="8">
+        <v>0.25368899999999989</v>
+      </c>
+      <c r="C6" s="9">
+        <v>0.25356200000000001</v>
+      </c>
+      <c r="D6" s="9">
         <v>0.252855</v>
       </c>
-      <c r="E6" s="10">
-        <v>0.256871</v>
-      </c>
-      <c r="F6" s="10">
-        <v>0.254613</v>
-      </c>
-      <c r="G6" s="10">
-        <v>0.25363</v>
-      </c>
-      <c r="H6" s="10">
-        <v>0.257275</v>
-      </c>
-      <c r="I6" s="10">
-        <v>0.255644</v>
+      <c r="E6" s="9">
+        <v>0.25687100000000002</v>
+      </c>
+      <c r="F6" s="9">
+        <v>0.25461299999999998</v>
+      </c>
+      <c r="G6" s="9">
+        <v>0.25363000000000002</v>
+      </c>
+      <c r="H6" s="9">
+        <v>0.25727499999999998</v>
+      </c>
+      <c r="I6" s="9">
+        <v>0.25564399999999998</v>
       </c>
     </row>
-    <row r="7" ht="21.35" customHeight="1">
-      <c r="A7" s="8">
+    <row r="7" spans="1:9" ht="21.3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
         <v>256</v>
       </c>
-      <c r="B7" s="9">
-        <v>1.992914</v>
-      </c>
-      <c r="C7" s="10">
+      <c r="B7" s="8">
+        <v>1.9929140000000001</v>
+      </c>
+      <c r="C7" s="9">
         <v>1.993692</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="9">
         <v>2.00644</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="9">
         <v>1.988629</v>
       </c>
-      <c r="F7" s="10">
-        <v>1.983709</v>
-      </c>
-      <c r="G7" s="10">
+      <c r="F7" s="9">
+        <v>1.9837089999999999</v>
+      </c>
+      <c r="G7" s="9">
         <v>1.985719</v>
       </c>
-      <c r="H7" s="10">
-        <v>1.98781</v>
-      </c>
-      <c r="I7" s="10">
+      <c r="H7" s="9">
+        <v>1.9878100000000001</v>
+      </c>
+      <c r="I7" s="9">
         <v>1.986963</v>
       </c>
     </row>
-    <row r="8" ht="21.35" customHeight="1">
-      <c r="A8" s="8">
+    <row r="8" spans="1:9" ht="21.3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
         <v>512</v>
       </c>
-      <c r="B8" s="9">
-        <v>16.74594099999999</v>
-      </c>
-      <c r="C8" s="10">
+      <c r="B8" s="8">
+        <v>16.745940999999991</v>
+      </c>
+      <c r="C8" s="9">
         <v>16.209847</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="9">
         <v>16.421135</v>
       </c>
-      <c r="E8" s="10">
-        <v>16.316598</v>
-      </c>
-      <c r="F8" s="10">
-        <v>16.268803</v>
-      </c>
-      <c r="G8" s="10">
+      <c r="E8" s="9">
+        <v>16.316597999999999</v>
+      </c>
+      <c r="F8" s="9">
+        <v>16.268802999999998</v>
+      </c>
+      <c r="G8" s="9">
         <v>16.560789</v>
       </c>
-      <c r="H8" s="10">
-        <v>16.720092</v>
-      </c>
-      <c r="I8" s="10">
-        <v>17.093817</v>
+      <c r="H8" s="9">
+        <v>16.720092000000001</v>
+      </c>
+      <c r="I8" s="9">
+        <v>17.093817000000001</v>
       </c>
     </row>
-    <row r="9" ht="21.35" customHeight="1">
-      <c r="A9" s="8">
+    <row r="9" spans="1:9" ht="21.3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
         <v>1024</v>
       </c>
-      <c r="B9" s="9">
-        <v>131.00549</v>
-      </c>
-      <c r="C9" s="10">
+      <c r="B9" s="8">
+        <v>131.00549000000001</v>
+      </c>
+      <c r="C9" s="9">
         <v>133.721689</v>
       </c>
-      <c r="D9" s="10">
-        <v>131.952509</v>
-      </c>
-      <c r="E9" s="10">
-        <v>134.846062</v>
-      </c>
-      <c r="F9" s="10">
+      <c r="D9" s="9">
+        <v>131.95250899999999</v>
+      </c>
+      <c r="E9" s="9">
+        <v>134.84606199999999</v>
+      </c>
+      <c r="F9" s="9">
         <v>134.381327</v>
       </c>
-      <c r="G9" s="10">
-        <v>133.66747</v>
-      </c>
-      <c r="H9" s="10">
-        <v>137.373101</v>
-      </c>
-      <c r="I9" s="10">
-        <v>139.850581</v>
+      <c r="G9" s="9">
+        <v>133.66747000000001</v>
+      </c>
+      <c r="H9" s="9">
+        <v>137.37310099999999</v>
+      </c>
+      <c r="I9" s="9">
+        <v>139.85058100000001</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:I1"/>
   </mergeCells>
-  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -2479,186 +2490,180 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:IV5"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B2" xSplit="1" ySplit="1" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.3516" style="12" customWidth="1"/>
-    <col min="2" max="2" width="16.3516" style="12" customWidth="1"/>
-    <col min="3" max="3" width="16.3516" style="12" customWidth="1"/>
-    <col min="4" max="4" width="16.3516" style="12" customWidth="1"/>
-    <col min="5" max="5" width="16.3516" style="12" customWidth="1"/>
-    <col min="6" max="6" width="16.3516" style="12" customWidth="1"/>
-    <col min="7" max="7" width="16.3516" style="12" customWidth="1"/>
-    <col min="8" max="8" width="16.3516" style="12" customWidth="1"/>
-    <col min="9" max="9" width="16.3516" style="12" customWidth="1"/>
-    <col min="10" max="256" width="16.3516" style="12" customWidth="1"/>
+    <col min="1" max="256" width="16.33203125" style="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="20.55" customHeight="1">
-      <c r="A1" t="s" s="3">
+    <row r="1" spans="1:9" ht="20.55" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="4">
+      <c r="B1" s="3">
         <v>60</v>
       </c>
-      <c r="C1" s="4">
+      <c r="C1" s="3">
         <v>61</v>
       </c>
-      <c r="D1" s="4">
+      <c r="D1" s="3">
         <v>62</v>
       </c>
-      <c r="E1" s="4">
+      <c r="E1" s="3">
         <v>63</v>
       </c>
-      <c r="F1" s="4">
+      <c r="F1" s="3">
         <v>64</v>
       </c>
-      <c r="G1" s="4">
+      <c r="G1" s="3">
         <v>65</v>
       </c>
-      <c r="H1" s="4">
+      <c r="H1" s="3">
         <v>66</v>
       </c>
-      <c r="I1" s="4">
+      <c r="I1" s="3">
         <v>67</v>
       </c>
     </row>
-    <row r="2" ht="21.55" customHeight="1">
-      <c r="A2" t="s" s="13">
+    <row r="2" spans="1:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="5">
+        <v>2.1381070000000002</v>
+      </c>
+      <c r="C2" s="6">
+        <v>2.1172089999999999</v>
+      </c>
+      <c r="D2" s="6">
+        <v>2.0982750000000001</v>
+      </c>
+      <c r="E2" s="6">
+        <v>2.104133</v>
+      </c>
+      <c r="F2" s="6">
+        <v>1.8801859999999999</v>
+      </c>
+      <c r="G2" s="6">
+        <v>1.881707</v>
+      </c>
+      <c r="H2" s="6">
+        <v>1.8880539999999999</v>
+      </c>
+      <c r="I2" s="6">
+        <v>1.88889</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="46.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="6">
-        <v>2.138107</v>
-      </c>
-      <c r="C2" s="7">
-        <v>2.117209</v>
-      </c>
-      <c r="D2" s="7">
-        <v>2.098275</v>
-      </c>
-      <c r="E2" s="7">
-        <v>2.104133</v>
-      </c>
-      <c r="F2" s="7">
-        <v>1.880186</v>
-      </c>
-      <c r="G2" s="7">
-        <v>1.881707</v>
-      </c>
-      <c r="H2" s="7">
-        <v>1.888054</v>
-      </c>
-      <c r="I2" s="7">
-        <v>1.88889</v>
+      <c r="B3" s="8">
+        <v>1.9929140000000001</v>
+      </c>
+      <c r="C3" s="9">
+        <v>1.993692</v>
+      </c>
+      <c r="D3" s="9">
+        <v>2.00644</v>
+      </c>
+      <c r="E3" s="9">
+        <v>1.988629</v>
+      </c>
+      <c r="F3" s="9">
+        <v>1.9837089999999999</v>
+      </c>
+      <c r="G3" s="9">
+        <v>1.985719</v>
+      </c>
+      <c r="H3" s="9">
+        <v>1.9878100000000001</v>
+      </c>
+      <c r="I3" s="9">
+        <v>1.986963</v>
       </c>
     </row>
-    <row r="3" ht="46.7" customHeight="1">
-      <c r="A3" t="s" s="14">
+    <row r="4" spans="1:9" ht="21.3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="9">
-        <v>1.992914</v>
-      </c>
-      <c r="C3" s="10">
-        <v>1.993692</v>
-      </c>
-      <c r="D3" s="10">
-        <v>2.00644</v>
-      </c>
-      <c r="E3" s="10">
-        <v>1.988629</v>
-      </c>
-      <c r="F3" s="10">
-        <v>1.983709</v>
-      </c>
-      <c r="G3" s="10">
-        <v>1.985719</v>
-      </c>
-      <c r="H3" s="10">
-        <v>1.98781</v>
-      </c>
-      <c r="I3" s="10">
-        <v>1.986963</v>
+      <c r="B4" s="8">
+        <f t="shared" ref="B4:I4" si="0">B2/B3</f>
+        <v>1.0728546239325933</v>
+      </c>
+      <c r="C4" s="9">
+        <f t="shared" si="0"/>
+        <v>1.0619539026088283</v>
+      </c>
+      <c r="D4" s="9">
+        <f t="shared" si="0"/>
+        <v>1.0457701202129144</v>
+      </c>
+      <c r="E4" s="9">
+        <f t="shared" si="0"/>
+        <v>1.0580822264987588</v>
+      </c>
+      <c r="F4" s="9">
+        <f t="shared" si="0"/>
+        <v>0.94781341416508169</v>
+      </c>
+      <c r="G4" s="9">
+        <f t="shared" si="0"/>
+        <v>0.94761998047054996</v>
+      </c>
+      <c r="H4" s="9">
+        <f t="shared" si="0"/>
+        <v>0.94981612930813297</v>
+      </c>
+      <c r="I4" s="9">
+        <f t="shared" si="0"/>
+        <v>0.95064175830148823</v>
       </c>
     </row>
-    <row r="4" ht="21.35" customHeight="1">
-      <c r="A4" t="s" s="14">
+    <row r="5" spans="1:9" ht="21.3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="9">
-        <f>B2/B3</f>
-        <v>1.072854623932593</v>
-      </c>
-      <c r="C4" s="10">
-        <f>C2/C3</f>
-        <v>1.061953902608828</v>
-      </c>
-      <c r="D4" s="10">
-        <f>D2/D3</f>
-        <v>1.045770120212914</v>
-      </c>
-      <c r="E4" s="10">
-        <f>E2/E3</f>
-        <v>1.058082226498759</v>
-      </c>
-      <c r="F4" s="10">
-        <f>F2/F3</f>
-        <v>0.9478134141650817</v>
-      </c>
-      <c r="G4" s="10">
-        <f>G2/G3</f>
-        <v>0.9476199804705502</v>
-      </c>
-      <c r="H4" s="10">
-        <f>H2/H3</f>
-        <v>0.9498161293081333</v>
-      </c>
-      <c r="I4" s="10">
-        <f>I2/I3</f>
-        <v>0.9506417583014884</v>
-      </c>
-    </row>
-    <row r="5" ht="21.35" customHeight="1">
-      <c r="A5" t="s" s="14">
-        <v>7</v>
-      </c>
-      <c r="B5" s="9">
+      <c r="B5" s="8">
         <v>1</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="9">
         <v>1</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="9">
         <v>1</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="9">
         <v>1</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="9">
         <v>1</v>
       </c>
-      <c r="G5" s="10">
+      <c r="G5" s="9">
         <v>1</v>
       </c>
-      <c r="H5" s="10">
+      <c r="H5" s="9">
         <v>1</v>
       </c>
-      <c r="I5" s="10">
+      <c r="I5" s="9">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>